<commit_message>
actualización de ValidarEstructura, ValoresEstructura202 y ErroresEstructura
</commit_message>
<xml_diff>
--- a/src/archivoExcel.xlsx
+++ b/src/archivoExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DESARROLLOS\ANGULARJS\res202\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC9B8159-A1A3-4226-9193-6FABE7AA685F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BAF7BDD-26A8-413E-AD2C-D9631AD31661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3658,7 +3658,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="173">
   <si>
     <t>CC</t>
   </si>
@@ -4209,6 +4209,18 @@
   </si>
   <si>
     <t>CAM&amp;LA</t>
+  </si>
+  <si>
+    <t>CC_</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>AB</t>
+  </si>
+  <si>
+    <t>Caa</t>
   </si>
 </sst>
 </file>
@@ -9543,8 +9555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DO11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10340,7 +10352,7 @@
         <v>54</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>0</v>
+        <v>169</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>163</v>
@@ -10698,9 +10710,7 @@
       <c r="C4" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>0</v>
-      </c>
+      <c r="D4" s="5"/>
       <c r="E4" s="5">
         <v>25516237</v>
       </c>
@@ -11058,7 +11068,7 @@
         <v>54</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>0</v>
+        <v>172</v>
       </c>
       <c r="E5" s="5">
         <v>76330054</v>
@@ -11776,7 +11786,7 @@
         <v>54</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="E7" s="5">
         <v>10525194</v>
@@ -12853,7 +12863,7 @@
         <v>54</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>0</v>
+        <v>171</v>
       </c>
       <c r="E10" s="5">
         <v>34522452</v>

</xml_diff>

<commit_message>
terminacion creacion validacionEstructura datos usuario
</commit_message>
<xml_diff>
--- a/src/archivoExcel.xlsx
+++ b/src/archivoExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DESARROLLOS\ANGULARJS\res202\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BAF7BDD-26A8-413E-AD2C-D9631AD31661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325FFD7E-B2E6-4C68-BD38-D7C662E6679F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3658,7 +3658,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="177">
   <si>
     <t>CC</t>
   </si>
@@ -4211,16 +4211,28 @@
     <t>CAM&amp;LA</t>
   </si>
   <si>
-    <t>CC_</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>AB</t>
-  </si>
-  <si>
-    <t>Caa</t>
+    <t>3</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13 </t>
   </si>
 </sst>
 </file>
@@ -9556,7 +9568,7 @@
   <dimension ref="A1:DO11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10016,8 +10028,8 @@
       <c r="K2" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="L2" s="7">
-        <v>6</v>
+      <c r="L2" s="7" t="s">
+        <v>169</v>
       </c>
       <c r="M2" s="7">
         <v>9999</v>
@@ -10352,7 +10364,7 @@
         <v>54</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>169</v>
+        <v>0</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>163</v>
@@ -10381,8 +10393,8 @@
       <c r="M3" s="8">
         <v>9999</v>
       </c>
-      <c r="N3" s="8">
-        <v>13</v>
+      <c r="N3" s="8" t="s">
+        <v>173</v>
       </c>
       <c r="O3" s="17">
         <v>0</v>
@@ -10710,7 +10722,9 @@
       <c r="C4" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="5"/>
+      <c r="D4" s="5" t="s">
+        <v>0</v>
+      </c>
       <c r="E4" s="5">
         <v>25516237</v>
       </c>
@@ -10738,8 +10752,8 @@
       <c r="M4" s="8">
         <v>9999</v>
       </c>
-      <c r="N4" s="8">
-        <v>13</v>
+      <c r="N4" s="8" t="s">
+        <v>176</v>
       </c>
       <c r="O4" s="17">
         <v>0</v>
@@ -11068,7 +11082,7 @@
         <v>54</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>172</v>
+        <v>0</v>
       </c>
       <c r="E5" s="5">
         <v>76330054</v>
@@ -11097,8 +11111,8 @@
       <c r="M5" s="8">
         <v>9999</v>
       </c>
-      <c r="N5" s="8">
-        <v>13</v>
+      <c r="N5" s="8" t="s">
+        <v>175</v>
       </c>
       <c r="O5" s="17">
         <v>0</v>
@@ -11450,14 +11464,14 @@
       <c r="K6" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="L6" s="8">
-        <v>6</v>
+      <c r="L6" s="8" t="s">
+        <v>170</v>
       </c>
       <c r="M6" s="8">
         <v>9999</v>
       </c>
-      <c r="N6" s="8">
-        <v>13</v>
+      <c r="N6" s="8" t="s">
+        <v>174</v>
       </c>
       <c r="O6" s="17">
         <v>21</v>
@@ -11786,7 +11800,7 @@
         <v>54</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>170</v>
+        <v>0</v>
       </c>
       <c r="E7" s="5">
         <v>10525194</v>
@@ -11809,8 +11823,8 @@
       <c r="K7" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="L7" s="8">
-        <v>6</v>
+      <c r="L7" s="8" t="s">
+        <v>171</v>
       </c>
       <c r="M7" s="8">
         <v>9999</v>
@@ -12863,7 +12877,7 @@
         <v>54</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>171</v>
+        <v>0</v>
       </c>
       <c r="E10" s="5">
         <v>34522452</v>
@@ -12886,8 +12900,8 @@
       <c r="K10" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="L10" s="8">
-        <v>6</v>
+      <c r="L10" s="8" t="s">
+        <v>172</v>
       </c>
       <c r="M10" s="8">
         <v>9999</v>

</xml_diff>